<commit_message>
Created 5 test cases for the Sauce Demo Website. Implemented custom data provider with .xlsx files. Implemented page objects for the test cases. Implemented a TopMenu AbstractUIObject. Configured properties files.
</commit_message>
<xml_diff>
--- a/src/test/resources/data_source/demo.xlsx
+++ b/src/test/resources/data_source/demo.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\IdeaProjects\test-automation\src\test\resources\data_source\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A70085-8F02-4659-B8DE-20909DE47670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="19425" yWindow="8700" windowWidth="17520" windowHeight="9825" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="GSMArena" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Data" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Calculator" sheetId="3" r:id="rId6"/>
+    <sheet name="GSMArena" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Calculator" sheetId="3" r:id="rId3"/>
+    <sheet name="Credentials" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Execute</t>
   </si>
@@ -196,43 +206,67 @@
   </si>
   <si>
     <t>XLS0003</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>shouldLogin</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Menlo"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -242,7 +276,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -258,58 +292,57 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -499,20 +532,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -564,7 +600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -590,7 +626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -617,21 +653,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -646,7 +683,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -661,7 +698,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -676,7 +713,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -691,7 +728,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -705,7 +742,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -719,7 +756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
@@ -733,7 +770,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -747,7 +784,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -762,27 +799,30 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.88"/>
-    <col customWidth="1" min="3" max="3" width="5.25"/>
-    <col customWidth="1" min="4" max="4" width="2.88"/>
-    <col customWidth="1" min="5" max="5" width="6.25"/>
+    <col min="1" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +839,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -807,16 +847,16 @@
         <v>58</v>
       </c>
       <c r="C2" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="7">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -824,16 +864,16 @@
         <v>59</v>
       </c>
       <c r="C3" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="7">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -841,40 +881,140 @@
         <v>60</v>
       </c>
       <c r="C4" s="2">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="D4" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="E4" s="7">
-        <v>116.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950DD170-90B2-468C-BB8F-490CF664DFC1}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>